<commit_message>
Updated Calibration for IR Sensors
</commit_message>
<xml_diff>
--- a/Lab2/Calibration.xlsx
+++ b/Lab2/Calibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leenb1\Desktop\Rose\2021-2022\ECE425\Lenardo-ECE425-2122\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE901E68-DDC6-4952-80D1-58B89AACEEC4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A6B526-FA10-43BF-B724-61A1F42F24AC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{3ACC7381-090E-421A-8FC4-756E8D653B23}"/>
   </bookViews>
@@ -25,12 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Distance</t>
   </si>
   <si>
-    <t>Output</t>
+    <t>k</t>
+  </si>
+  <si>
+    <t>m'</t>
+  </si>
+  <si>
+    <t>b'</t>
+  </si>
+  <si>
+    <t>Output (Front,Back)</t>
+  </si>
+  <si>
+    <t>Output (Left,Right)</t>
   </si>
 </sst>
 </file>
@@ -160,122 +172,24 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$B$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>530</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>490</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>330</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>65</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$C$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4BDB-421D-BFD0-94DC7C1DBA26}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.1300349956255468"/>
-                  <c:y val="-1.7351633129192183E-2"/>
+                  <c:x val="-0.35883661417322832"/>
+                  <c:y val="1.8101851851851852E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -310,114 +224,138 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$18</c:f>
+              <c:f>Sheet1!$B$3:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>530</c:v>
+                  <c:v>667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>490</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>330</c:v>
+                  <c:v>368</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>245</c:v>
+                  <c:v>272</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>200</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>160</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>135</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>120</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>110</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>95</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>90</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>85</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>65</c:v>
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$18</c:f>
+              <c:f>Sheet1!$D$3:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.70422535211267612</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41322314049586778</c:v>
+                  <c:v>0.2857142857142857</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.29239766081871343</c:v>
+                  <c:v>0.22222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.22624434389140272</c:v>
+                  <c:v>0.18181818181818182</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18450184501845018</c:v>
+                  <c:v>0.15384615384615385</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1557632398753894</c:v>
+                  <c:v>0.13333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13477088948787061</c:v>
+                  <c:v>0.11764705882352941</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.11876484560570072</c:v>
+                  <c:v>0.10526315789473684</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.10615711252653928</c:v>
+                  <c:v>9.5238095238095233E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.5969289827255277E-2</c:v>
+                  <c:v>8.6956521739130432E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.7565674255691769E-2</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.0515297906602251E-2</c:v>
+                  <c:v>7.407407407407407E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.4515648286140088E-2</c:v>
+                  <c:v>6.8965517241379309E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.9348127600554782E-2</c:v>
+                  <c:v>6.4516129032258063E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.4850843060959798E-2</c:v>
+                  <c:v>6.0606060606060608E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.0901339829476243E-2</c:v>
+                  <c:v>5.7142857142857141E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.4054054054054057E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.128205128205128E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.878048780487805E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.6511627906976744E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -425,7 +363,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4BDB-421D-BFD0-94DC7C1DBA26}"/>
+              <c16:uniqueId val="{00000000-4BDB-421D-BFD0-94DC7C1DBA26}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -698,7 +636,7 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -712,11 +650,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -726,20 +664,20 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="power"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.0760498687664045E-2"/>
-                  <c:y val="-0.39409303003791191"/>
+                  <c:x val="-0.27798293963254594"/>
+                  <c:y val="-7.8546952464275302E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -774,108 +712,135 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$18</c:f>
+              <c:f>Sheet1!$B$28:$B$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>593</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>670</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>560</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>449</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>388</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>343</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>308</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15</c:v>
+                  <c:v>187</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16</c:v>
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$18</c:f>
+              <c:f>Sheet1!$D$28:$D$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>490</c:v>
-                </c:pt>
+                <c:ptCount val="20"/>
                 <c:pt idx="1">
-                  <c:v>330</c:v>
+                  <c:v>0.26315789473684209</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>245</c:v>
+                  <c:v>0.20833333333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>200</c:v>
+                  <c:v>0.17241379310344829</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>160</c:v>
+                  <c:v>0.14705882352941177</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>150</c:v>
+                  <c:v>0.12820512820512822</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>135</c:v>
+                  <c:v>0.11363636363636363</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>120</c:v>
+                  <c:v>0.1020408163265306</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>110</c:v>
+                  <c:v>9.2592592592592587E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>8.4745762711864403E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>95</c:v>
+                  <c:v>7.8125E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>90</c:v>
+                  <c:v>7.2463768115942032E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>85</c:v>
+                  <c:v>6.7567567567567557E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>70</c:v>
+                  <c:v>6.3291139240506319E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>65</c:v>
+                  <c:v>5.9523809523809521E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.6179775280898875E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.3191489361702128E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.0505050505050504E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.8076923076923073E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.5871559633027519E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -883,7 +848,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-DF7B-4FFC-8925-5E2FBFEB72D9}"/>
+              <c16:uniqueId val="{00000001-1763-485C-81A3-6D656979B044}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -895,11 +860,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="346442704"/>
-        <c:axId val="346439096"/>
+        <c:axId val="406910920"/>
+        <c:axId val="406912560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="346442704"/>
+        <c:axId val="406910920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,12 +921,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346439096"/>
+        <c:crossAx val="406912560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="346439096"/>
+        <c:axId val="406912560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1018,7 +983,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346442704"/>
+        <c:crossAx val="406910920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1030,6 +995,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2192,12 +2188,12 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>179070</xdr:rowOff>
     </xdr:to>
@@ -2227,22 +2223,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE6666DA-160E-41C5-8683-9FC94BF033A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F92057D2-1C9C-4584-BD2E-4F491DBCE330}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2560,232 +2556,549 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A91262CB-2F0B-4C23-AE63-C1EA4ACB5925}">
-  <dimension ref="A2:D22"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="C24" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <f>(1.5+1.5)/2</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>530</v>
+        <v>667</v>
       </c>
       <c r="D3">
-        <f>1/(A3+0.42)</f>
-        <v>0.70422535211267612</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <f>1/(A3+$D$1)</f>
+        <v>0.4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <f>1/0.0005</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>490</v>
+        <v>512</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D18" si="0">1/(A4+0.42)</f>
-        <v>0.41322314049586778</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" ref="D4:D22" si="0">1/(A4+$D$1)</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <f>0.0249/0.0005</f>
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>330</v>
+        <v>368</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0.29239766081871343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0.22624434389140272</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.18181818181818182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.18450184501845018</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.15384615384615385</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0.1557632398753894</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.13477088948787061</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.11764705882352941</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0.11876484560570072</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.10526315789473684</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>0.10615711252653928</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9.5238095238095233E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>9.5969289827255277E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8.6956521739130432E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>8.7565674255691769E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>8.0515297906602251E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.407407407407407E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>7.4515648286140088E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6.8965517241379309E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>6.9348127600554782E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6.4516129032258063E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>6.4850843060959798E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6.0606060606060608E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>6.0901339829476243E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.7142857142857141E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>57</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>5.4054054054054057E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>56</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>5.128205128205128E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>55</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>4.878048780487805E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
+      </c>
+      <c r="B22">
+        <v>54</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>4.6511627906976744E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>593</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <f>1/0.0004</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>670</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ref="D29:D47" si="1">1/(A29+$D$26)</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="F29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <f>-0.0129/0.0004</f>
+        <v>-32.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>560</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>449</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>0.17241379310344829</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>388</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>0.14705882352941177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>343</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>0.12820512820512822</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <v>308</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>0.11363636363636363</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>280</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>0.1020408163265306</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36">
+        <v>255</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>9.2592592592592587E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>240</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>8.4745762711864403E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>11</v>
+      </c>
+      <c r="B38">
+        <v>223</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>7.8125E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39">
+        <v>207</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>7.2463768115942032E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <v>196</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>6.7567567567567557E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>14</v>
+      </c>
+      <c r="B41">
+        <v>187</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>6.3291139240506319E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>180</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>5.9523809523809521E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>16</v>
+      </c>
+      <c r="B43">
+        <v>170</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>5.6179775280898875E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>17</v>
+      </c>
+      <c r="B44">
+        <v>164</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>5.3191489361702128E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>18</v>
+      </c>
+      <c r="B45">
+        <v>157</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>5.0505050505050504E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>19</v>
+      </c>
+      <c r="B46">
+        <v>153</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>4.8076923076923073E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>20</v>
+      </c>
+      <c r="B47">
+        <v>144</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>4.5871559633027519E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>